<commit_message>
en14015 add method to plot data, update data.
</commit_message>
<xml_diff>
--- a/utilityscripts/loads/en14015_data.xlsx
+++ b/utilityscripts/loads/en14015_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\loads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57AC412F-1BD6-4A6B-962A-DA4191CF9DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6609BC1B-DE5C-4630-B443-C25C9237C671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-270" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{A44FF89C-7D98-49A8-8A66-57688544CD45}"/>
+    <workbookView xWindow="28680" yWindow="-270" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{A44FF89C-7D98-49A8-8A66-57688544CD45}"/>
   </bookViews>
   <sheets>
     <sheet name="t1-tt" sheetId="2" r:id="rId1"/>
@@ -52,6 +52,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -81,8 +84,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,13 +421,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C577C9-BA1D-4AC7-83C0-CCD66D81F469}">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -434,491 +441,331 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>-5.1515009600366902E-4</v>
-      </c>
-      <c r="B2">
-        <v>1.0015542953522101</v>
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0.16842286017577501</v>
-      </c>
-      <c r="B3">
-        <v>0.96802053613382</v>
+      <c r="A3" s="1">
+        <v>0.19999999999999901</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.95890214323158596</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0.30053544388766601</v>
-      </c>
-      <c r="B4">
-        <v>0.94037040888241896</v>
+      <c r="A4" s="1">
+        <v>0.39999999999999902</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.917741207251352</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0.42635695218470399</v>
-      </c>
-      <c r="B5">
-        <v>0.91328517126582998</v>
+      <c r="A5" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.87703074736475295</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>0.55846953589659498</v>
-      </c>
-      <c r="B6">
-        <v>0.88395994505062703</v>
+      <c r="A6" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.83496731569957505</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>0.696873195023338</v>
-      </c>
-      <c r="B7">
-        <v>0.85775572660634103</v>
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.78740711668646202</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0.82898577873522805</v>
-      </c>
-      <c r="B8">
-        <v>0.82910760031275799</v>
+      <c r="A8" s="1">
+        <v>1.19999999999999</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.73390363939713898</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>0.94851621161741495</v>
-      </c>
-      <c r="B9">
-        <v>0.80087345325985204</v>
+      <c r="A9" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.68514994051230704</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1.05546449366989</v>
-      </c>
-      <c r="B10">
-        <v>0.77267226176709403</v>
+      <c r="A10" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.63854908478629802</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1.1624127757223801</v>
-      </c>
-      <c r="B11">
-        <v>0.74440757791074896</v>
+      <c r="A11" s="1">
+        <v>1.7999999999999901</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.59572050084304595</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1.2756521331897099</v>
-      </c>
-      <c r="B12">
-        <v>0.71508821534817102</v>
+      <c r="A12" s="1">
+        <v>1.99999999999999</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.55558988808425303</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1.38260041524219</v>
-      </c>
-      <c r="B13">
-        <v>0.68842281682824402</v>
+      <c r="A13" s="1">
+        <v>2.19999999999999</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.51754731566391599</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1.4958397727095301</v>
-      </c>
-      <c r="B14">
-        <v>0.66050889470770902</v>
+      <c r="A14" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.48004229222561201</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1.62166128100657</v>
-      </c>
-      <c r="B15">
-        <v>0.63298288069422504</v>
+      <c r="A15" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.44665241435972802</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1.75377386471846</v>
-      </c>
-      <c r="B16">
-        <v>0.60433187977404201</v>
+      <c r="A16" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.415415363991681</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1.8921775238452001</v>
-      </c>
-      <c r="B17">
-        <v>0.576795434087918</v>
+      <c r="A17" s="1">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.38614215594837498</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2.03058118297194</v>
-      </c>
-      <c r="B18">
-        <v>0.54985077217771205</v>
+      <c r="A18" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.35982095219124399</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2.1626937666838302</v>
-      </c>
-      <c r="B19">
-        <v>0.52464780906706598</v>
+      <c r="A19" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.33582522114539798</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2.2948063503957199</v>
-      </c>
-      <c r="B20">
-        <v>0.49849588170932002</v>
+      <c r="A20" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.31314527537280301</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2.4332100095224698</v>
-      </c>
-      <c r="B21">
-        <v>0.47521534839447199</v>
+      <c r="A21" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.29395065259479403</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2.5716136686492099</v>
-      </c>
-      <c r="B22">
-        <v>0.45158849309642901</v>
+      <c r="A22" s="1">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.27675972375360902</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2.7100173277759501</v>
-      </c>
-      <c r="B23">
-        <v>0.42891594726319199</v>
+      <c r="A23" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.26292484319428899</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2.8484209869026902</v>
-      </c>
-      <c r="B24">
-        <v>0.40729775946768598</v>
+      <c r="A24" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.25079503823720201</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>2.9696671676252899</v>
-      </c>
-      <c r="B25">
-        <v>0.38919956972175102</v>
+      <c r="A25" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.240469707530129</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>3.0990961457406399</v>
-      </c>
-      <c r="B26">
-        <v>0.37323447640594298</v>
+      <c r="A26" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.23180650310242701</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>3.2316926583306</v>
-      </c>
-      <c r="B27">
-        <v>0.35768373135535397</v>
+      <c r="A27" s="1">
+        <v>5</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.223179082422129</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>3.3584820243837701</v>
-      </c>
-      <c r="B28">
-        <v>0.33996521311692302</v>
+      <c r="A28" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.21493238305012999</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>3.4901106792175902</v>
-      </c>
-      <c r="B29">
-        <v>0.32555752567190599</v>
+      <c r="A29" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.20784035214751001</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>3.6285143383443299</v>
-      </c>
-      <c r="B30">
-        <v>0.31221313497018399</v>
+      <c r="A30" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.20095315529282101</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>3.7669179974710798</v>
-      </c>
-      <c r="B31">
-        <v>0.299399221591929</v>
+      <c r="A31" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.19442303555450499</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>3.9053216565978199</v>
-      </c>
-      <c r="B32">
-        <v>0.28629670656101103</v>
+      <c r="A32" s="1">
+        <v>6</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.18873815796749299</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>4.0437253157245596</v>
-      </c>
-      <c r="B33">
-        <v>0.27659969103152099</v>
+      <c r="A33" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.182900954247914</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>4.1821289748512998</v>
-      </c>
-      <c r="B34">
-        <v>0.26459386228072301</v>
+      <c r="A34" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.17643428141443099</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>4.3205326339780497</v>
-      </c>
-      <c r="B35">
-        <v>0.257263380303073</v>
+      <c r="A35" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.171467095189894</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>4.4589362931047898</v>
-      </c>
-      <c r="B36">
-        <v>0.248143568078909</v>
+      <c r="A36" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.166299335414684</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>4.5973399522315299</v>
-      </c>
-      <c r="B37">
-        <v>0.241448009737119</v>
+      <c r="A37" s="1">
+        <v>7</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.16113991884915799</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>4.73574361135827</v>
-      </c>
-      <c r="B38">
-        <v>0.235655113338571</v>
+      <c r="A38" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.155058683917321</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>4.8741472704850199</v>
-      </c>
-      <c r="B39">
-        <v>0.23080822880892801</v>
+      <c r="A39" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.15076157606828799</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>5.0125509296117601</v>
-      </c>
-      <c r="B40">
-        <v>0.22378558859411901</v>
+      <c r="A40" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.14595067278738399</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>5.1509545887385002</v>
-      </c>
-      <c r="B41">
-        <v>0.21870619950724299</v>
+      <c r="A41" s="1">
+        <v>7.8</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.142642373017631</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>5.2893582478652403</v>
-      </c>
-      <c r="B42">
-        <v>0.212818725792909</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>5.4277619069919902</v>
-      </c>
-      <c r="B43">
-        <v>0.207894880822556</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>5.5661655661187304</v>
-      </c>
-      <c r="B44">
-        <v>0.202198184974896</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>5.7045692252454696</v>
-      </c>
-      <c r="B45">
-        <v>0.198042321176543</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>5.8429728843722097</v>
-      </c>
-      <c r="B46">
-        <v>0.193193813411798</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>5.9813765434989596</v>
-      </c>
-      <c r="B47">
-        <v>0.18913577339943499</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>6.1197802026256998</v>
-      </c>
-      <c r="B48">
-        <v>0.18507529853441901</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>6.2581838617524399</v>
-      </c>
-      <c r="B49">
-        <v>0.18153430664419701</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>6.39658752087918</v>
-      </c>
-      <c r="B50">
-        <v>0.17818652747330099</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>6.5349911800059299</v>
-      </c>
-      <c r="B51">
-        <v>0.17376049051491199</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>6.6733948391326701</v>
-      </c>
-      <c r="B52">
-        <v>0.17022112185979199</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>6.8117984982594102</v>
-      </c>
-      <c r="B53">
-        <v>0.16660479276396101</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>6.9502021573861601</v>
-      </c>
-      <c r="B54">
-        <v>0.16317924153480501</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>7.0886058165129002</v>
-      </c>
-      <c r="B55">
-        <v>0.16006234368604</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>7.2270094756396404</v>
-      </c>
-      <c r="B56">
-        <v>0.15717632715940599</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>7.3654131347663796</v>
-      </c>
-      <c r="B57">
-        <v>0.15305894358140801</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>7.5038167938931197</v>
-      </c>
-      <c r="B58">
-        <v>0.14986752014458599</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>7.6422204530198696</v>
-      </c>
-      <c r="B59">
-        <v>0.146634370017205</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>7.7806241121466098</v>
-      </c>
-      <c r="B60">
-        <v>0.14317033856769301</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>7.9190277712733499</v>
-      </c>
-      <c r="B61">
-        <v>0.14166960997384301</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>7.9945206762515797</v>
-      </c>
-      <c r="B62">
-        <v>0.140324425496516</v>
+      <c r="A42" s="1">
+        <v>8</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.138198757763969</v>
       </c>
     </row>
   </sheetData>
@@ -1063,17 +910,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B6E431-F425-41EC-9EED-16702BDB3E0D}">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1085,499 +930,331 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>-3.81679389312994E-3</v>
-      </c>
-      <c r="B2">
-        <v>1.07858243451461E-2</v>
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>9.1476461074717595E-3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0.13740458015267201</v>
-      </c>
-      <c r="B3">
-        <v>3.8520801232665602E-2</v>
+      <c r="A3" s="1">
+        <v>0.19999999999999901</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4.8095009094471897E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0.26315905465825101</v>
-      </c>
-      <c r="B4">
-        <v>6.6711039960616697E-2</v>
+      <c r="A4" s="1">
+        <v>0.39999999999999902</v>
+      </c>
+      <c r="B4" s="1">
+        <v>9.3716534523752101E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0.39210554159273298</v>
-      </c>
-      <c r="B5">
-        <v>9.5783969348144593E-2</v>
+      <c r="A5" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.139406347146773</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>0.52072308340748397</v>
-      </c>
-      <c r="B6">
-        <v>0.12673605096445301</v>
+      <c r="A6" s="1">
+        <v>0.79999999999999905</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.185836322086814</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>0.66442449025199601</v>
-      </c>
-      <c r="B7">
-        <v>0.160258146761214</v>
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.233208548384748</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0.80354795205778395</v>
-      </c>
-      <c r="B8">
-        <v>0.18618039284024701</v>
+      <c r="A8" s="1">
+        <v>1.19999999999999</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.27878003144707902</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>0.87073564285197302</v>
-      </c>
-      <c r="B9">
-        <v>0.209596699600197</v>
+      <c r="A9" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.32170840669227802</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>0.99395175628023502</v>
-      </c>
-      <c r="B10">
-        <v>0.23107437995310101</v>
+      <c r="A10" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.36153625881407803</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1.07666157193155</v>
-      </c>
-      <c r="B11">
-        <v>0.25536528375629602</v>
+      <c r="A11" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.39902116680057198</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1.16572386804598</v>
-      </c>
-      <c r="B12">
-        <v>0.27648383928490899</v>
+      <c r="A12" s="1">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.43355699700245798</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1.29123003421696</v>
-      </c>
-      <c r="B13">
-        <v>0.30202752431098101</v>
+      <c r="A13" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.46603101815833597</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1.40134615484683</v>
-      </c>
-      <c r="B14">
-        <v>0.32168600321610602</v>
+      <c r="A14" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.49695925068117602</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1.5068491546855201</v>
-      </c>
-      <c r="B15">
-        <v>0.34617911463601397</v>
+      <c r="A15" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.52384484597157299</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1.6396956971958101</v>
-      </c>
-      <c r="B16">
-        <v>0.36910129433993299</v>
+      <c r="A16" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.54959839909606201</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1.7617204862951099</v>
-      </c>
-      <c r="B17">
-        <v>0.39083810922878698</v>
+      <c r="A17" s="1">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.57299964270706905</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1.90327942163612</v>
-      </c>
-      <c r="B18">
-        <v>0.41693181594214601</v>
+      <c r="A18" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.59416522359693702</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2.0362431508453098</v>
-      </c>
-      <c r="B19">
-        <v>0.43852930364264398</v>
+      <c r="A19" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.61441399203190505</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2.1359566961707102</v>
-      </c>
-      <c r="B20">
-        <v>0.460176226757541</v>
+      <c r="A20" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.63225917540939602</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2.26964204873632</v>
-      </c>
-      <c r="B21">
-        <v>0.48288291082774298</v>
+      <c r="A21" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.64884133095005203</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2.4042710626141499</v>
-      </c>
-      <c r="B22">
-        <v>0.49669212138017299</v>
+      <c r="A22" s="1">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.66266255107490901</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2.5070252943900599</v>
-      </c>
-      <c r="B23">
-        <v>0.51658821762388396</v>
+      <c r="A23" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.67601068290175403</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2.6501023238249801</v>
-      </c>
-      <c r="B24">
-        <v>0.53472959015227906</v>
+      <c r="A24" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.68776038437797204</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>2.7765229821615298</v>
-      </c>
-      <c r="B25">
-        <v>0.55132294138221105</v>
+      <c r="A25" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.698289342357024</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>2.89335723986592</v>
-      </c>
-      <c r="B26">
-        <v>0.56131814052311901</v>
+      <c r="A26" s="1">
+        <v>4.7999999999999901</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.70714221213812101</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>3.0349328697900702</v>
-      </c>
-      <c r="B27">
-        <v>0.58043688850409803</v>
+      <c r="A27" s="1">
+        <v>4.9999999999999902</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.71581360601812305</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>3.1784604817433899</v>
-      </c>
-      <c r="B28">
-        <v>0.59279180491616801</v>
+      <c r="A28" s="1">
+        <v>5.1999999999999904</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.72290361306873097</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>3.3196225354751001</v>
-      </c>
-      <c r="B29">
-        <v>0.60595240120871696</v>
+      <c r="A29" s="1">
+        <v>5.3999999999999897</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.72969347046341304</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>3.4641075675028699</v>
-      </c>
-      <c r="B30">
-        <v>0.62096299527307097</v>
+      <c r="A30" s="1">
+        <v>5.5999999999999899</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.73507636700896195</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>3.5907678858552199</v>
-      </c>
-      <c r="B31">
-        <v>0.63125360393999197</v>
+      <c r="A31" s="1">
+        <v>5.7999999999999901</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.74080633267596396</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>3.7371181665586199</v>
-      </c>
-      <c r="B32">
-        <v>0.64231166378296101</v>
+      <c r="A32" s="1">
+        <v>5.9999999999999902</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.74654239864244298</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>3.8743502084016299</v>
-      </c>
-      <c r="B33">
-        <v>0.65481942525719095</v>
+      <c r="A33" s="1">
+        <v>6.1999999999999904</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.751487406945755</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>4.0049303506663101</v>
-      </c>
-      <c r="B34">
-        <v>0.66616450206447098</v>
+      <c r="A34" s="1">
+        <v>6.3999999999999897</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.75658108890148001</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>4.14677912252023</v>
-      </c>
-      <c r="B35">
-        <v>0.67623044369430996</v>
+      <c r="A35" s="1">
+        <v>6.5999999999999899</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.76022473140118296</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>4.2962081830812204</v>
-      </c>
-      <c r="B36">
-        <v>0.68299598354345104</v>
+      <c r="A36" s="1">
+        <v>6.7999999999999901</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.76460259544054099</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>4.4268518084890403</v>
-      </c>
-      <c r="B37">
-        <v>0.69224627474705402</v>
+      <c r="A37" s="1">
+        <v>6.9999999999999902</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.768357460458719</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>4.56273903744985</v>
-      </c>
-      <c r="B38">
-        <v>0.70084517316242401</v>
+      <c r="A38" s="1">
+        <v>7.1999999999999904</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.77250986712608305</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>4.7009929090667102</v>
-      </c>
-      <c r="B39">
-        <v>0.70781854103056197</v>
+      <c r="A39" s="1">
+        <v>7.3999999999999897</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.77643303448785495</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>4.8364008179958997</v>
-      </c>
-      <c r="B40">
-        <v>0.71267363244591098</v>
+      <c r="A40" s="1">
+        <v>7.5999999999999801</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.778969195477202</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>4.9748044771226496</v>
-      </c>
-      <c r="B41">
-        <v>0.717333587130915</v>
+      <c r="A41" s="1">
+        <v>7.7999999999999803</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.782024771053762</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>5.1132081362493897</v>
-      </c>
-      <c r="B42">
-        <v>0.72202748175221099</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>5.2418256780641403</v>
-      </c>
-      <c r="B43">
-        <v>0.72678782557123001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>5.39001545450287</v>
-      </c>
-      <c r="B44">
-        <v>0.73206107985428703</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>5.5284191136296199</v>
-      </c>
-      <c r="B45">
-        <v>0.73665471583693998</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>5.66682277275636</v>
-      </c>
-      <c r="B46">
-        <v>0.74155738372749902</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>5.7997453736225797</v>
-      </c>
-      <c r="B47">
-        <v>0.74394984470891701</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>5.9424983218595298</v>
-      </c>
-      <c r="B48">
-        <v>0.74702923309557401</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>6.0820337501365902</v>
-      </c>
-      <c r="B49">
-        <v>0.74877204651657103</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>6.2166206153701999</v>
-      </c>
-      <c r="B50">
-        <v>0.75355279376425599</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>6.3666853993974204</v>
-      </c>
-      <c r="B51">
-        <v>0.75774118432951698</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>6.4972447275168204</v>
-      </c>
-      <c r="B52">
-        <v>0.76194744400785797</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>6.6375841021558202</v>
-      </c>
-      <c r="B53">
-        <v>0.764130333174733</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>6.7761490709085797</v>
-      </c>
-      <c r="B54">
-        <v>0.76666938626749304</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>6.9095521316286499</v>
-      </c>
-      <c r="B55">
-        <v>0.77006500483676299</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>7.0508593640237898</v>
-      </c>
-      <c r="B56">
-        <v>0.77171981663554301</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>7.1902308809066602</v>
-      </c>
-      <c r="B57">
-        <v>0.77409669114982604</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>7.33465676607155</v>
-      </c>
-      <c r="B58">
-        <v>0.77740680171791698</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>7.4631667681356202</v>
-      </c>
-      <c r="B59">
-        <v>0.78107412904127005</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>7.6056057696810697</v>
-      </c>
-      <c r="B60">
-        <v>0.78194848940309103</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>7.7554598104872001</v>
-      </c>
-      <c r="B61">
-        <v>0.78478303982855602</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>7.8824130879345597</v>
-      </c>
-      <c r="B62">
-        <v>0.78661600781804597</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>7.9850840631292996</v>
-      </c>
-      <c r="B63">
-        <v>0.78668744516722</v>
+      <c r="A42" s="1">
+        <v>8</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.783004068989406</v>
       </c>
     </row>
   </sheetData>
@@ -2092,7 +1769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4522F5EF-414D-48D6-87EF-ED4BDCE8730E}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>